<commit_message>
updated mod perf wksht
</commit_message>
<xml_diff>
--- a/Model Performance Worksheet.xlsx
+++ b/Model Performance Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danrk\Desktop\Data Bootcamp\Project 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDA6F00-B19B-472F-8143-B88916F8F94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2190E2-EFFE-4ADC-A985-DBEDB9164828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{A17727D7-62F3-485D-A4D5-CB5FDCB6B5B2}"/>
   </bookViews>
@@ -66,44 +66,48 @@
     <t>None</t>
   </si>
   <si>
-    <t>Activation Function: Relu
+    <t>Model Notes</t>
+  </si>
+  <si>
+    <t>Estimators - 500
+Successfully found at least some of classes 0 through 6
+successful classes had at 350+ instances in the testing data
+65%+ precision per successful class (exception: class 4, 42%)
+Poor recall except for class 0, 1</t>
+  </si>
+  <si>
+    <t>Optimizations</t>
+  </si>
+  <si>
+    <t>Best k: 16</t>
+  </si>
+  <si>
+    <t>Max iteration: 30,000</t>
+  </si>
+  <si>
+    <t>80%/20% train/test split
+multi-class solver 'ovr' used
+model only predicted class 0 (No playable hand) for all testing data</t>
+  </si>
+  <si>
+    <t>Reasonable precision/recall scores for classes 0, 1 (60% +)
+Steep drop off in performance for remaining classes
+(Scores of 35% or less for precision and recall)</t>
+  </si>
+  <si>
+    <t>K curve optimal k values: 6, 16
+Suprising performance on class 5 (Flush: 99% recall! Only 29% precision)
+Generally poor performance except for class 0 precision/recall 
+(moderate performance of 75%/60%)</t>
+  </si>
+  <si>
+    <t>Superior performance in comparison to tested models
+Activation Function: Relu
 Initial Layer: 21 neurons
 1st Hidden Layer: 41 neurons
 2nd Hidden Layer: 21 neurons
 Output Layer: 10 neurons, SoftMax Activation Function
 Testing Loss: 0.0132</t>
-  </si>
-  <si>
-    <t>Model Notes</t>
-  </si>
-  <si>
-    <t>80/20 train/test split
-multi-class solver 'ovr' used
-model only predicted class 0 (No playable hand) for all testing data</t>
-  </si>
-  <si>
-    <t>Estimators - 500
-Successfully found at least some of classes 0 through 6
-successful classes had at 350+ instances in the testing data
-65%+ precision per successful class (exception: class 4, 42%)
-Poor recall except for class 0, 1</t>
-  </si>
-  <si>
-    <t>Reasonable precision/recall scores for classes 0,1 (60% +)
-Steep drop off in performance for remaining classes
-(Scores of 35% or less for precision and recall)</t>
-  </si>
-  <si>
-    <t>Optimizations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Determined max iterations: </t>
-  </si>
-  <si>
-    <t>K curve optimal k values: 6, 16</t>
-  </si>
-  <si>
-    <t>Best k: 16</t>
   </si>
 </sst>
 </file>
@@ -147,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -161,9 +165,6 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -485,7 +486,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +494,7 @@
     <col min="1" max="1" width="34.140625" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="64.5703125" customWidth="1"/>
+    <col min="4" max="4" width="67.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -504,14 +505,14 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5">
@@ -521,22 +522,22 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="5">
         <v>0.50119999999999998</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5">
@@ -546,25 +547,25 @@
         <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>0.56999999999999995</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="5">
@@ -574,10 +575,10 @@
         <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -588,7 +589,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>